<commit_message>
Made further UI changes and fixed some issues for NREGA data.
</commit_message>
<xml_diff>
--- a/Input File/NREGADataApril062011ForTool.xlsx
+++ b/Input File/NREGADataApril062011ForTool.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="203">
   <si>
     <t>No. of Disabled beneficiary individuals</t>
   </si>
@@ -565,45 +565,21 @@
     <t>Udupi Chikmagalur</t>
   </si>
   <si>
-    <t>HHs Jobcards - SCs+STs</t>
-  </si>
-  <si>
     <t xml:space="preserve">No of SC households issued job cards </t>
   </si>
   <si>
     <t xml:space="preserve">No of ST households issued job cards </t>
   </si>
   <si>
-    <t xml:space="preserve">No of households issued job cards </t>
-  </si>
-  <si>
     <t xml:space="preserve">No of households demanded employment </t>
   </si>
   <si>
-    <t>No of households provided employment</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> No of households completed 100 days</t>
-  </si>
-  <si>
     <t>Percentage SC / STs employed (w.r.t total persondays)</t>
   </si>
   <si>
-    <t>Percentage women employed (w.r.t total persondays)</t>
-  </si>
-  <si>
-    <t>Percentage SC/ST Job cards issued (w.r.t total job cards issued)</t>
-  </si>
-  <si>
-    <t>Wage per personday (in Rs.)</t>
-  </si>
-  <si>
     <t>Expenditure  on material  (in Lakhs Rs.)</t>
   </si>
   <si>
-    <t>Expenditure on unskilled wages (in Lakhs Rs.)</t>
-  </si>
-  <si>
     <t>Year</t>
   </si>
   <si>
@@ -617,6 +593,37 @@
   </si>
   <si>
     <t>Total Constituency Population</t>
+  </si>
+  <si>
+    <t>Total job cards issued</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The data above shows that the percentage of employment to women with respect to total employment provided in Bilgi constituency is lower than the neighbouring constituencies such as Chittapur and Gurmitkal. Is this government data correct? Can this be brought to the government’s notice? 
+</t>
+  </si>
+  <si>
+    <t>SC/ST Job Cards Issued</t>
+  </si>
+  <si>
+    <t>Employment Provided</t>
+  </si>
+  <si>
+    <t>% Women Employed (w.r.t total Person Days)</t>
+  </si>
+  <si>
+    <t>% SC/ST Job cards issued (w.r.t total job cards)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> No of families completed 100 days</t>
+  </si>
+  <si>
+    <t>Average Daily Wate (in Rs.)</t>
+  </si>
+  <si>
+    <t>Expenditure on wages (in Lakhs Rs.)</t>
   </si>
 </sst>
 </file>
@@ -714,7 +721,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -747,6 +754,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1049,11 +1059,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R170"/>
+  <dimension ref="A1:S159"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1073,65 +1083,69 @@
     <col min="16" max="16" width="12.5703125" style="12" customWidth="1"/>
     <col min="17" max="17" width="12.7109375" style="12" customWidth="1"/>
     <col min="18" max="18" width="12.85546875" style="12" customWidth="1"/>
+    <col min="19" max="19" width="36.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="63" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="52.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="H1" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="I1" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>196</v>
-      </c>
-      <c r="D1" s="11" t="s">
+      <c r="J1" s="11" t="s">
         <v>200</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="K1" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="P1" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q1" s="11" t="s">
         <v>186</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>191</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="K1" s="11" t="s">
-        <v>193</v>
-      </c>
-      <c r="L1" s="11" t="s">
-        <v>195</v>
-      </c>
-      <c r="M1" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="N1" s="11" t="s">
-        <v>184</v>
-      </c>
-      <c r="O1" s="11" t="s">
-        <v>185</v>
-      </c>
-      <c r="P1" s="11" t="s">
-        <v>187</v>
-      </c>
-      <c r="Q1" s="11" t="s">
-        <v>190</v>
       </c>
       <c r="R1" s="11" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S1" s="11" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="135" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
@@ -1139,7 +1153,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D2" s="13">
         <v>245036</v>
@@ -1187,8 +1201,11 @@
       <c r="R2" s="12">
         <v>53</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S2" s="15" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>2</v>
       </c>
@@ -1196,7 +1213,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D3" s="13">
         <v>240739</v>
@@ -1245,7 +1262,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>2</v>
       </c>
@@ -1253,7 +1270,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D4" s="13">
         <v>228554</v>
@@ -1302,7 +1319,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>2</v>
       </c>
@@ -1310,7 +1327,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D5" s="13">
         <v>215353</v>
@@ -1359,7 +1376,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>2</v>
       </c>
@@ -1367,7 +1384,7 @@
         <v>79</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D6" s="13">
         <v>219559</v>
@@ -1416,7 +1433,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>2</v>
       </c>
@@ -1424,7 +1441,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D7" s="13">
         <v>239708</v>
@@ -1473,7 +1490,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>169</v>
       </c>
@@ -1481,7 +1498,7 @@
         <v>21</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D8" s="13">
         <v>262653</v>
@@ -1530,7 +1547,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>169</v>
       </c>
@@ -1538,7 +1555,7 @@
         <v>16</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D9" s="13">
         <v>213924</v>
@@ -1587,7 +1604,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>169</v>
       </c>
@@ -1595,7 +1612,7 @@
         <v>14</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D10" s="13">
         <v>255946</v>
@@ -1644,7 +1661,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>169</v>
       </c>
@@ -1652,7 +1669,7 @@
         <v>24</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D11" s="13">
         <v>227412</v>
@@ -1701,7 +1718,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>169</v>
       </c>
@@ -1709,7 +1726,7 @@
         <v>26</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D12" s="13">
         <v>224309</v>
@@ -1758,7 +1775,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>181</v>
       </c>
@@ -1766,7 +1783,7 @@
         <v>29</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D13" s="13">
         <v>201328</v>
@@ -1815,7 +1832,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>181</v>
       </c>
@@ -1823,7 +1840,7 @@
         <v>30</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D14" s="13">
         <v>224658</v>
@@ -1872,7 +1889,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>181</v>
       </c>
@@ -1880,7 +1897,7 @@
         <v>27</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D15" s="13">
         <v>241625</v>
@@ -1929,7 +1946,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>181</v>
       </c>
@@ -1937,7 +1954,7 @@
         <v>31</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D16" s="13">
         <v>218747</v>
@@ -1994,7 +2011,7 @@
         <v>28</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D17" s="13">
         <v>210959</v>
@@ -2051,7 +2068,7 @@
         <v>7</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D18" s="13">
         <v>230054</v>
@@ -2108,7 +2125,7 @@
         <v>8</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D19" s="13">
         <v>246115</v>
@@ -2165,7 +2182,7 @@
         <v>135</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D20" s="13">
         <v>252574</v>
@@ -2222,7 +2239,7 @@
         <v>136</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D21" s="13">
         <v>246962</v>
@@ -2279,7 +2296,7 @@
         <v>147</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D22" s="13">
         <v>236030</v>
@@ -2336,7 +2353,7 @@
         <v>137</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D23" s="13">
         <v>257322</v>
@@ -2393,7 +2410,7 @@
         <v>83</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D24" s="13">
         <v>238563</v>
@@ -2450,7 +2467,7 @@
         <v>34</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D25" s="13">
         <v>245294</v>
@@ -2507,7 +2524,7 @@
         <v>35</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D26" s="13">
         <v>252353</v>
@@ -2564,7 +2581,7 @@
         <v>37</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D27" s="13">
         <v>257042</v>
@@ -2621,7 +2638,7 @@
         <v>38</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D28" s="13">
         <v>228308</v>
@@ -2678,7 +2695,7 @@
         <v>85</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D29" s="13">
         <v>225294</v>
@@ -2735,7 +2752,7 @@
         <v>36</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D30" s="13">
         <v>279133</v>
@@ -2792,7 +2809,7 @@
         <v>42</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D31" s="13">
         <v>204748</v>
@@ -2849,7 +2866,7 @@
         <v>39</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D32" s="13">
         <v>224217</v>
@@ -2906,7 +2923,7 @@
         <v>40</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D33" s="13">
         <v>219003</v>
@@ -2963,7 +2980,7 @@
         <v>43</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D34" s="13">
         <v>239776</v>
@@ -3020,7 +3037,7 @@
         <v>45</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D35" s="13">
         <v>224185</v>
@@ -3077,7 +3094,7 @@
         <v>41</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D36" s="13">
         <v>242411</v>
@@ -3134,7 +3151,7 @@
         <v>44</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D37" s="13">
         <v>230197</v>
@@ -3191,7 +3208,7 @@
         <v>47</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D38" s="13">
         <v>242924</v>
@@ -3248,7 +3265,7 @@
         <v>48</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D39" s="13">
         <v>240045</v>
@@ -3305,7 +3322,7 @@
         <v>120</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D40" s="13">
         <v>245930</v>
@@ -3362,7 +3379,7 @@
         <v>46</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D41" s="13">
         <v>244974</v>
@@ -3419,7 +3436,7 @@
         <v>125</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D42" s="13">
         <v>237698</v>
@@ -3476,7 +3493,7 @@
         <v>127</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D43" s="13">
         <v>224250</v>
@@ -3533,7 +3550,7 @@
         <v>123</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D44" s="13">
         <v>246706</v>
@@ -3590,7 +3607,7 @@
         <v>49</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D45" s="13">
         <v>221517</v>
@@ -3647,7 +3664,7 @@
         <v>50</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D46" s="13">
         <v>230847</v>
@@ -3704,7 +3721,7 @@
         <v>9</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D47" s="13">
         <v>226390</v>
@@ -3761,7 +3778,7 @@
         <v>53</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D48" s="13">
         <v>231394</v>
@@ -3818,7 +3835,7 @@
         <v>10</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D49" s="13">
         <v>222430</v>
@@ -3875,7 +3892,7 @@
         <v>11</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D50" s="13">
         <v>211751</v>
@@ -3932,7 +3949,7 @@
         <v>12</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D51" s="13">
         <v>243302</v>
@@ -3989,7 +4006,7 @@
         <v>19</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D52" s="13">
         <v>239081</v>
@@ -4046,7 +4063,7 @@
         <v>22</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D53" s="13">
         <v>228725</v>
@@ -4103,7 +4120,7 @@
         <v>13</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D54" s="13">
         <v>218560</v>
@@ -4160,7 +4177,7 @@
         <v>25</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D55" s="13">
         <v>208796</v>
@@ -4217,7 +4234,7 @@
         <v>18</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D56" s="13">
         <v>249235</v>
@@ -4274,7 +4291,7 @@
         <v>20</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D57" s="13">
         <v>218089</v>
@@ -4331,7 +4348,7 @@
         <v>15</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D58" s="13">
         <v>219668</v>
@@ -4388,7 +4405,7 @@
         <v>60</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D59" s="13">
         <v>240129</v>
@@ -4445,7 +4462,7 @@
         <v>62</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D60" s="13">
         <v>264719</v>
@@ -4502,7 +4519,7 @@
         <v>61</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D61" s="13">
         <v>267910</v>
@@ -4559,7 +4576,7 @@
         <v>63</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D62" s="13">
         <v>219445</v>
@@ -4616,7 +4633,7 @@
         <v>59</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D63" s="13">
         <v>266412</v>
@@ -4673,7 +4690,7 @@
         <v>149</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D64" s="13">
         <v>246255</v>
@@ -4730,7 +4747,7 @@
         <v>150</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D65" s="13">
         <v>256561</v>
@@ -4787,7 +4804,7 @@
         <v>64</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D66" s="13">
         <v>238788</v>
@@ -4844,7 +4861,7 @@
         <v>67</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D67" s="13">
         <v>246494</v>
@@ -4901,7 +4918,7 @@
         <v>66</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D68" s="13">
         <v>224879</v>
@@ -4958,7 +4975,7 @@
         <v>68</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D69" s="13">
         <v>220090</v>
@@ -5015,7 +5032,7 @@
         <v>65</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D70" s="13">
         <v>233723</v>
@@ -5072,7 +5089,7 @@
         <v>69</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D71" s="13">
         <v>236117</v>
@@ -5129,7 +5146,7 @@
         <v>70</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D72" s="13">
         <v>215915</v>
@@ -5186,7 +5203,7 @@
         <v>73</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D73" s="13">
         <v>245654</v>
@@ -5243,7 +5260,7 @@
         <v>74</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D74" s="13">
         <v>222592</v>
@@ -5300,7 +5317,7 @@
         <v>72</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D75" s="13">
         <v>208085</v>
@@ -5357,7 +5374,7 @@
         <v>71</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D76" s="13">
         <v>230278</v>
@@ -5414,7 +5431,7 @@
         <v>76</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D77" s="13">
         <v>216792</v>
@@ -5471,7 +5488,7 @@
         <v>78</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D78" s="13">
         <v>219666</v>
@@ -5528,7 +5545,7 @@
         <v>77</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D79" s="13">
         <v>242415</v>
@@ -5585,7 +5602,7 @@
         <v>100</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D80" s="13">
         <v>250759</v>
@@ -5642,7 +5659,7 @@
         <v>82</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D81" s="13">
         <v>229899</v>
@@ -5699,7 +5716,7 @@
         <v>87</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D82" s="13">
         <v>245900</v>
@@ -5756,7 +5773,7 @@
         <v>84</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D83" s="13">
         <v>278340</v>
@@ -5813,7 +5830,7 @@
         <v>166</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D84" s="13">
         <v>230027</v>
@@ -5870,7 +5887,7 @@
         <v>88</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D85" s="13">
         <v>235254</v>
@@ -5927,7 +5944,7 @@
         <v>86</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D86" s="13">
         <v>243998</v>
@@ -5984,7 +6001,7 @@
         <v>91</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D87" s="13">
         <v>266197</v>
@@ -6041,7 +6058,7 @@
         <v>92</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D88" s="13">
         <v>250448</v>
@@ -6098,7 +6115,7 @@
         <v>93</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D89" s="13">
         <v>236351</v>
@@ -6155,7 +6172,7 @@
         <v>95</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D90" s="13">
         <v>250144</v>
@@ -6212,7 +6229,7 @@
         <v>56</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D91" s="13">
         <v>237019</v>
@@ -6269,7 +6286,7 @@
         <v>90</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D92" s="13">
         <v>259954</v>
@@ -6326,7 +6343,7 @@
         <v>94</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D93" s="13">
         <v>235016</v>
@@ -6383,7 +6400,7 @@
         <v>96</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D94" s="13">
         <v>236858</v>
@@ -6440,7 +6457,7 @@
         <v>97</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D95" s="13">
         <v>230750</v>
@@ -6497,7 +6514,7 @@
         <v>98</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D96" s="13">
         <v>256397</v>
@@ -6554,7 +6571,7 @@
         <v>99</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D97" s="13">
         <v>212458</v>
@@ -6611,7 +6628,7 @@
         <v>80</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D98" s="13">
         <v>263136</v>
@@ -6668,7 +6685,7 @@
         <v>81</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D99" s="13">
         <v>238835</v>
@@ -6725,7 +6742,7 @@
         <v>104</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D100" s="13">
         <v>212879</v>
@@ -6782,7 +6799,7 @@
         <v>51</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D101" s="13">
         <v>238087</v>
@@ -6839,7 +6856,7 @@
         <v>106</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D102" s="13">
         <v>207009</v>
@@ -6896,7 +6913,7 @@
         <v>107</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D103" s="13">
         <v>231302</v>
@@ -6953,7 +6970,7 @@
         <v>52</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D104" s="13">
         <v>227162</v>
@@ -7010,7 +7027,7 @@
         <v>105</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D105" s="13">
         <v>239004</v>
@@ -7067,7 +7084,7 @@
         <v>109</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D106" s="13">
         <v>219795</v>
@@ -7124,7 +7141,7 @@
         <v>110</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D107" s="13">
         <v>248994</v>
@@ -7181,7 +7198,7 @@
         <v>108</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D108" s="13">
         <v>251596</v>
@@ -7238,7 +7255,7 @@
         <v>111</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D109" s="13">
         <v>239331</v>
@@ -7295,7 +7312,7 @@
         <v>132</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D110" s="13">
         <v>222494</v>
@@ -7352,7 +7369,7 @@
         <v>134</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D111" s="13">
         <v>256128</v>
@@ -7409,7 +7426,7 @@
         <v>32</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D112" s="13">
         <v>235344</v>
@@ -7466,7 +7483,7 @@
         <v>112</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D113" s="13">
         <v>236373</v>
@@ -7523,7 +7540,7 @@
         <v>122</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D114" s="13">
         <v>239199</v>
@@ -7580,7 +7597,7 @@
         <v>114</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D115" s="13">
         <v>248245</v>
@@ -7637,7 +7654,7 @@
         <v>115</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D116" s="13">
         <v>242935</v>
@@ -7694,7 +7711,7 @@
         <v>117</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D117" s="13">
         <v>281809</v>
@@ -7751,7 +7768,7 @@
         <v>119</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D118" s="13">
         <v>237512</v>
@@ -7808,7 +7825,7 @@
         <v>116</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D119" s="13">
         <v>238618</v>
@@ -7865,7 +7882,7 @@
         <v>118</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D120" s="13">
         <v>245160</v>
@@ -7922,7 +7939,7 @@
         <v>124</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D121" s="13">
         <v>236846</v>
@@ -7979,7 +7996,7 @@
         <v>121</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D122" s="13">
         <v>253926</v>
@@ -8036,7 +8053,7 @@
         <v>101</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D123" s="13">
         <v>272478</v>
@@ -8093,7 +8110,7 @@
         <v>126</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D124" s="13">
         <v>224254</v>
@@ -8150,7 +8167,7 @@
         <v>102</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D125" s="13">
         <v>276083</v>
@@ -8207,7 +8224,7 @@
         <v>129</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D126" s="13">
         <v>222457</v>
@@ -8264,7 +8281,7 @@
         <v>131</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D127" s="13">
         <v>247104</v>
@@ -8321,7 +8338,7 @@
         <v>133</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D128" s="13">
         <v>252188</v>
@@ -8378,7 +8395,7 @@
         <v>130</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D129" s="13">
         <v>242987</v>
@@ -8435,7 +8452,7 @@
         <v>164</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D130" s="13">
         <v>223247</v>
@@ -8492,7 +8509,7 @@
         <v>165</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D131" s="13">
         <v>273984</v>
@@ -8549,7 +8566,7 @@
         <v>163</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D132" s="13">
         <v>228922</v>
@@ -8606,7 +8623,7 @@
         <v>155</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D133" s="13">
         <v>244883</v>
@@ -8663,7 +8680,7 @@
         <v>140</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D134" s="13">
         <v>232026</v>
@@ -8720,7 +8737,7 @@
         <v>142</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D135" s="13">
         <v>213590</v>
@@ -8777,7 +8794,7 @@
         <v>138</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D136" s="13">
         <v>250243</v>
@@ -8834,7 +8851,7 @@
         <v>141</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D137" s="13">
         <v>215767</v>
@@ -8891,7 +8908,7 @@
         <v>139</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D138" s="13">
         <v>221488</v>
@@ -8948,7 +8965,7 @@
         <v>143</v>
       </c>
       <c r="C139" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D139" s="13">
         <v>254534</v>
@@ -9005,7 +9022,7 @@
         <v>144</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D140" s="13">
         <v>211919</v>
@@ -9062,7 +9079,7 @@
         <v>146</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D141" s="13">
         <v>237019</v>
@@ -9119,7 +9136,7 @@
         <v>148</v>
       </c>
       <c r="C142" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D142" s="13">
         <v>232017</v>
@@ -9176,7 +9193,7 @@
         <v>151</v>
       </c>
       <c r="C143" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D143" s="13">
         <v>217124</v>
@@ -9233,7 +9250,7 @@
         <v>152</v>
       </c>
       <c r="C144" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D144" s="13">
         <v>225532</v>
@@ -9290,7 +9307,7 @@
         <v>145</v>
       </c>
       <c r="C145" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D145" s="13">
         <v>218791</v>
@@ -9347,7 +9364,7 @@
         <v>156</v>
       </c>
       <c r="C146" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D146" s="13">
         <v>205541</v>
@@ -9404,7 +9421,7 @@
         <v>153</v>
       </c>
       <c r="C147" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D147" s="13">
         <v>205598</v>
@@ -9461,7 +9478,7 @@
         <v>154</v>
       </c>
       <c r="C148" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D148" s="13">
         <v>224574</v>
@@ -9518,7 +9535,7 @@
         <v>54</v>
       </c>
       <c r="C149" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D149" s="13">
         <v>224546</v>
@@ -9575,7 +9592,7 @@
         <v>55</v>
       </c>
       <c r="C150" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D150" s="13">
         <v>206495</v>
@@ -9632,7 +9649,7 @@
         <v>57</v>
       </c>
       <c r="C151" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D151" s="13">
         <v>224170</v>
@@ -9689,7 +9706,7 @@
         <v>158</v>
       </c>
       <c r="C152" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D152" s="13">
         <v>247861</v>
@@ -9746,7 +9763,7 @@
         <v>159</v>
       </c>
       <c r="C153" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D153" s="13">
         <v>208055</v>
@@ -9803,7 +9820,7 @@
         <v>157</v>
       </c>
       <c r="C154" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D154" s="13">
         <v>249439</v>
@@ -9860,7 +9877,7 @@
         <v>23</v>
       </c>
       <c r="C155" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D155" s="13">
         <v>243185</v>
@@ -9917,7 +9934,7 @@
         <v>17</v>
       </c>
       <c r="C156" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D156" s="13">
         <v>229746</v>
@@ -9974,7 +9991,7 @@
         <v>160</v>
       </c>
       <c r="C157" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D157" s="13">
         <v>207634</v>
@@ -10031,7 +10048,7 @@
         <v>162</v>
       </c>
       <c r="C158" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D158" s="13">
         <v>232649</v>
@@ -10088,7 +10105,7 @@
         <v>161</v>
       </c>
       <c r="C159" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D159" s="13">
         <v>208006</v>
@@ -10136,42 +10153,6 @@
       <c r="R159" s="12">
         <v>51</v>
       </c>
-    </row>
-    <row r="160" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C160" s="3"/>
-      <c r="D160" s="13">
-        <v>37198946</v>
-      </c>
-    </row>
-    <row r="161" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C161" s="3"/>
-    </row>
-    <row r="162" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C162" s="3"/>
-    </row>
-    <row r="163" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C163" s="3"/>
-    </row>
-    <row r="164" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C164" s="3"/>
-    </row>
-    <row r="165" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C165" s="3"/>
-    </row>
-    <row r="166" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C166" s="3"/>
-    </row>
-    <row r="167" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C167" s="3"/>
-    </row>
-    <row r="168" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C168" s="3"/>
-    </row>
-    <row r="169" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C169" s="3"/>
-    </row>
-    <row r="170" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C170" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>